<commit_message>
Added new test case for Utilization endpoint: lastLogin by equipmentId
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Utilization.xlsx
+++ b/src/test/resources/data/Activity_Utilization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DA87A4-65E2-4BC1-88EE-AF807131DCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FBDC57-53B2-43AE-8018-891B63077FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="17490" windowHeight="9180" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17490" windowHeight="9180" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_equipment" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>getEquipmentSurvey.json</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get random equipmentId</t>
+  </si>
+  <si>
+    <t>Get Last Logins by Equipment ID</t>
   </si>
 </sst>
 </file>
@@ -471,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FFDFA5-5332-432A-9925-5010622BDC15}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,38 +550,227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE10D00-541A-4267-9151-85470916DD6A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="6" max="6" width="54.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F63CBE-20C6-4938-94A8-B06668624B57}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="36.36328125" customWidth="1"/>
+    <col min="6" max="6" width="54.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="36.36328125" customWidth="1"/>
+    <col min="6" max="6" width="54.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed happy path scenarios for the utilization feature
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Utilization.xlsx
+++ b/src/test/resources/data/Activity_Utilization.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FBDC57-53B2-43AE-8018-891B63077FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4FD6E-CE70-4987-BF4C-080330373EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="17490" windowHeight="9180" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17490" windowHeight="9180" firstSheet="1" activeTab="3" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_equipment" sheetId="9" r:id="rId1"/>
-    <sheet name="GET_equipId_sessions" sheetId="11" r:id="rId2"/>
-    <sheet name="GET_equipId_summary" sheetId="12" r:id="rId3"/>
-    <sheet name="GET_equipId_last_login" sheetId="10" r:id="rId4"/>
+    <sheet name="GET_last_login" sheetId="11" r:id="rId2"/>
+    <sheet name="GET_equipment_session" sheetId="12" r:id="rId3"/>
+    <sheet name="GET_equipment_summary" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>TCID</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Get Last Logins by Equipment ID</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/sessions?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/summary?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get equipment session</t>
   </si>
 </sst>
 </file>
@@ -552,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE10D00-541A-4267-9151-85470916DD6A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -629,8 +638,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F63CBE-20C6-4938-94A8-B06668624B57}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="54.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,87 +766,14 @@
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="36.36328125" customWidth="1"/>
-    <col min="6" max="6" width="54.08984375" customWidth="1"/>
-    <col min="8" max="8" width="20.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
finished schema validations for all happy paths
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Utilization.xlsx
+++ b/src/test/resources/data/Activity_Utilization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9402462A-E4C1-4327-8CF0-FA07120789EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585A9AAC-2105-4A10-9001-B0B0F21B627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="440" windowWidth="19160" windowHeight="9760" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="26145" yWindow="-18570" windowWidth="23685" windowHeight="16395" activeTab="3" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_equipment" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Get equipment activity survey</t>
   </si>
   <si>
-    <t>getEquipmentSurvey.json</t>
-  </si>
-  <si>
     <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
   </si>
   <si>
@@ -104,6 +101,15 @@
   </si>
   <si>
     <t>GET_equipment.json</t>
+  </si>
+  <si>
+    <t>GET_last_login.json</t>
+  </si>
+  <si>
+    <t>GET_equipment_session.json</t>
+  </si>
+  <si>
+    <t>GET_equipment_summary.json</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,7 +558,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -613,21 +619,23 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
   </sheetData>
@@ -639,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F63CBE-20C6-4938-94A8-B06668624B57}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -688,25 +696,28 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -714,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,23 +777,24 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished adding tests for utilization
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Utilization.xlsx
+++ b/src/test/resources/data/Activity_Utilization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3332612-410D-41AA-BD0B-F5FF49D9986C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B280C4B9-2813-46A4-BF6F-FA42881FC365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_equipment" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>TCID</t>
   </si>
@@ -151,30 +151,12 @@
     <t>Get User Activity with startTimeStamp and endTimeStamp queries</t>
   </si>
   <si>
-    <t>Get user sessions using invalid userId and valid equipmentId</t>
-  </si>
-  <si>
     <t>Get equipment sessions, filter by locationId</t>
   </si>
   <si>
-    <t>Get equipment sessions, filter by equipmentTypeId</t>
-  </si>
-  <si>
     <t>Get last login, filter by userId</t>
   </si>
   <si>
-    <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;userId={userId}</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;locationId={locationId}</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;userId=bfc105b5-7ae6-432d-ae13-db2a3096a0c9</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/bfc105b5-7ae6-000d-ae13-db2a3096a0c9/last-logins?pageSize=50&amp;startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
-  </si>
-  <si>
     <t>/activity/v1/equipment/{equipmentId}/last-logins</t>
   </si>
   <si>
@@ -205,15 +187,9 @@
     <t>/activity/v1/equipment?startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;equipmentTypeId</t>
   </si>
   <si>
-    <t>/activity/v1/equipment/bfc105b5-7ae6-432d-ae13-db2a3096a000/last-logins?startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;userId={userId}</t>
-  </si>
-  <si>
     <t>/activity/v1/equipment/{equipmentId}/last-logins?startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
   </si>
   <si>
-    <t>/activity/v1/equipment/{equipmentId}/last-logins?startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=1</t>
-  </si>
-  <si>
     <t>/activity/v1/equipment/{equipmentId}/sessions</t>
   </si>
   <si>
@@ -229,21 +205,9 @@
     <t>/activity/v1/equipment/{equipmentId}/sessions&amp;locationId={locationId}</t>
   </si>
   <si>
-    <t>/activity/v1/equipment/{equipmentId}/sessions&amp;equipmentTypeId={equipmentTypeId}</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/{equipmentId}/sessions&amp;userId={userId0}</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/{equipmentId0}/sessions&amp;userId={userId}</t>
-  </si>
-  <si>
     <t>/activity/v1/equipment/{equipmentId}/sessions?startTimestamp=2021-5-1&amp;endTimestamp=2022-5-1</t>
   </si>
   <si>
-    <t>Get equipment sessions with valid userId and invalid equipmentId</t>
-  </si>
-  <si>
     <t>Get equipmentId sessions with startTimeStamp and endTimeStamp queries</t>
   </si>
   <si>
@@ -259,16 +223,46 @@
     <t>Get Equipment Summary, filter by equipmentId</t>
   </si>
   <si>
-    <t>/activity/v1/equipment/{equipmentId}/summary&amp;equipmentTypeId</t>
-  </si>
-  <si>
-    <t>/activity/v1/equipment/{equipmentId}/summary&amp;equipmentId</t>
-  </si>
-  <si>
     <t>Get Equipment Summary, filter by locationId</t>
   </si>
   <si>
     <t>/activity/v1/equipment/{equipmentId}/summary&amp;locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/last-logins?pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/bfc105b5-7ae6-432d-ae13-db2a3096a000/last-logins?userId={userId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/last-logins?userId=bfc105b5-7ae6-432d-ae13-db2a3096a0c9</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/last-logins?locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/last-logins?userId={userId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/bfc105b5-7ae6-000d-ae13-db2a3096a0c9/last-logins</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}0/sessions&amp;userId={userId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/sessions&amp;userId={userId}0</t>
+  </si>
+  <si>
+    <t>Get equipment sessions with invalid equipmentId and valid userId query</t>
+  </si>
+  <si>
+    <t>Get user sessions using valid euipmentId and invalid userId</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/summary&amp;equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/equipment/{equipmentId}/summary&amp;equipmentId={equipmentId}</t>
   </si>
 </sst>
 </file>
@@ -667,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FFDFA5-5332-432A-9925-5010622BDC15}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D12"/>
     </sheetView>
   </sheetViews>
@@ -722,7 +716,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
@@ -745,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>400</v>
@@ -768,7 +762,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>400</v>
@@ -791,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>400</v>
@@ -814,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G6">
         <v>200</v>
@@ -834,13 +828,13 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="G7">
         <v>200</v>
@@ -860,13 +854,13 @@
         <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>200</v>
@@ -886,13 +880,13 @@
         <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G9">
         <v>200</v>
@@ -922,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE10D00-541A-4267-9151-85470916DD6A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,7 +975,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>11</v>
@@ -992,7 +986,7 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1005,7 +999,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>23</v>
@@ -1015,20 +1009,23 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="G4" s="7">
         <v>200</v>
@@ -1038,20 +1035,23 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="G5" s="7">
         <v>200</v>
@@ -1061,20 +1061,23 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="G6" s="7">
         <v>400</v>
@@ -1084,20 +1087,23 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>7</v>
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G7" s="7">
         <v>400</v>
@@ -1107,20 +1113,23 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>8</v>
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G8" s="7">
         <v>200</v>
@@ -1130,20 +1139,23 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>10</v>
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G9" s="7">
         <v>200</v>
@@ -1159,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F63CBE-20C6-4938-94A8-B06668624B57}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1219,7 +1231,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
@@ -1243,7 +1255,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>23</v>
@@ -1260,16 +1272,22 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1280,96 +1298,98 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
+      <c r="C6" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>404</v>
+      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>67</v>
+      <c r="C8" t="s">
+        <v>56</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1382,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1441,7 +1461,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
@@ -1459,10 +1479,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1485,10 +1505,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1505,10 +1525,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1519,16 +1539,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>